<commit_message>
Finally able to parse JSON to get answer object in js file. TheSolicita mas info buton link was updated in temario.php. Price per hour changed in course_prices.xlsx
</commit_message>
<xml_diff>
--- a/admin/course_prices.xlsx
+++ b/admin/course_prices.xlsx
@@ -331,6 +331,76 @@
   <dxfs count="15">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -345,7 +415,20 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -383,160 +466,77 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -566,7 +566,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:M4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:M4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -581,29 +581,29 @@
     <filterColumn colId="12" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Curso" dataDxfId="13"/>
-    <tableColumn id="2" name="Total Unidades" dataDxfId="12"/>
-    <tableColumn id="3" name="Horas por Unidad" dataDxfId="11"/>
-    <tableColumn id="8" name="Horas semana" dataDxfId="10" dataCellStyle="Moneda"/>
-    <tableColumn id="12" name="Horas quincena" dataDxfId="1" dataCellStyle="Moneda"/>
-    <tableColumn id="13" name="Horas mes" dataDxfId="0" dataCellStyle="Moneda"/>
-    <tableColumn id="5" name="Total Horas" dataDxfId="9">
+    <tableColumn id="1" name="Curso" dataDxfId="12"/>
+    <tableColumn id="2" name="Total Unidades" dataDxfId="11"/>
+    <tableColumn id="3" name="Horas por Unidad" dataDxfId="10"/>
+    <tableColumn id="8" name="Horas semana" dataDxfId="9" dataCellStyle="Moneda"/>
+    <tableColumn id="12" name="Horas quincena" dataDxfId="8" dataCellStyle="Moneda"/>
+    <tableColumn id="13" name="Horas mes" dataDxfId="7" dataCellStyle="Moneda"/>
+    <tableColumn id="5" name="Total Horas" dataDxfId="6">
       <calculatedColumnFormula>Tabla1[Horas por Unidad]*Tabla1[Total Unidades]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Total Semanas" dataDxfId="2">
+    <tableColumn id="11" name="Total Semanas" dataDxfId="5">
       <calculatedColumnFormula>Tabla1[[#This Row],[Total Horas]]/Tabla1[[#This Row],[Horas semana]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Precio por hora" dataDxfId="3" dataCellStyle="Moneda"/>
-    <tableColumn id="6" name="Precio Total" dataDxfId="8" dataCellStyle="Moneda">
+    <tableColumn id="4" name="Precio por hora" dataDxfId="4" dataCellStyle="Moneda"/>
+    <tableColumn id="6" name="Precio Total" dataDxfId="3" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Total Horas]*Tabla1[Precio por hora]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Precio Semanal" dataDxfId="7" dataCellStyle="Moneda">
+    <tableColumn id="7" name="Precio Semanal" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Mensual" dataDxfId="6" dataCellStyle="Moneda">
+    <tableColumn id="9" name="Mensual" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Quincenal" dataDxfId="5" dataCellStyle="Moneda">
+    <tableColumn id="10" name="Quincenal" dataDxfId="0" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -877,7 +877,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2:M4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -964,23 +964,23 @@
         <v>36</v>
       </c>
       <c r="I2" s="4">
-        <v>72.5</v>
+        <v>50</v>
       </c>
       <c r="J2" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
-        <v>10440</v>
+        <v>7200</v>
       </c>
       <c r="K2" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="L2" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
-        <v>1160</v>
+        <v>800</v>
       </c>
       <c r="M2" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
-        <v>580</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1011,23 +1011,23 @@
         <v>36</v>
       </c>
       <c r="I3" s="4">
-        <v>72.5</v>
+        <v>50</v>
       </c>
       <c r="J3" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
-        <v>10440</v>
+        <v>7200</v>
       </c>
       <c r="K3" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="L3" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
-        <v>1160</v>
+        <v>800</v>
       </c>
       <c r="M3" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
-        <v>580</v>
+        <v>400</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1058,23 +1058,23 @@
         <v>24</v>
       </c>
       <c r="I4" s="4">
-        <v>72.5</v>
+        <v>50</v>
       </c>
       <c r="J4" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
-        <v>6960</v>
+        <v>4800</v>
       </c>
       <c r="K4" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="L4" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
-        <v>1160</v>
+        <v>800</v>
       </c>
       <c r="M4" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
-        <v>580</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1097,15 +1097,15 @@
         <v>0.3</v>
       </c>
       <c r="H9" s="6">
-        <f>J2-(L2*0.3)</f>
-        <v>10092</v>
+        <f>J2-(L2*G9)</f>
+        <v>6960</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J9" s="11">
         <f>J2-H9</f>
-        <v>348</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1113,15 +1113,15 @@
         <v>0.2</v>
       </c>
       <c r="H10" s="6">
-        <f>L2-(L3*0.2)</f>
-        <v>928</v>
+        <f>L2-(L3*G10)</f>
+        <v>640</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J10" s="11">
         <f>L2-H10</f>
-        <v>232</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1129,15 +1129,15 @@
         <v>0.1</v>
       </c>
       <c r="H11" s="6">
-        <f>M2-(M2*0.1)</f>
-        <v>522</v>
+        <f>M2-(M2*G11)</f>
+        <v>360</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="J11" s="11">
         <f>M2-H11</f>
-        <v>58</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1145,8 +1145,8 @@
         <v>0</v>
       </c>
       <c r="H12" s="13">
-        <f>K2-(K2*0)</f>
-        <v>290</v>
+        <f>K2-(K2*G12)</f>
+        <v>200</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Payment and Discount logic.
</commit_message>
<xml_diff>
--- a/admin/course_prices.xlsx
+++ b/admin/course_prices.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Curso</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Horas mes</t>
+  </si>
+  <si>
+    <t>Sem / unidad</t>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +139,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,7 +298,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,81 +331,40 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -415,6 +383,60 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -447,7 +469,6 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -471,58 +492,98 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -566,12 +627,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:M4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:N4" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N4">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
     <filterColumn colId="6" hiddenButton="1"/>
     <filterColumn colId="7" hiddenButton="1"/>
     <filterColumn colId="8" hiddenButton="1"/>
@@ -579,31 +642,39 @@
     <filterColumn colId="10" hiddenButton="1"/>
     <filterColumn colId="11" hiddenButton="1"/>
     <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="13">
-    <tableColumn id="1" name="Curso" dataDxfId="12"/>
-    <tableColumn id="2" name="Total Unidades" dataDxfId="11"/>
-    <tableColumn id="3" name="Horas por Unidad" dataDxfId="10"/>
+  <tableColumns count="14">
+    <tableColumn id="1" name="Curso" dataDxfId="3"/>
+    <tableColumn id="2" name="Total Unidades" dataDxfId="2"/>
+    <tableColumn id="3" name="Horas por Unidad" dataDxfId="0"/>
+    <tableColumn id="14" name="Sem / unidad" dataDxfId="1">
+      <calculatedColumnFormula>Tabla1[[#This Row],[Total Semanas]]/Tabla1[[#This Row],[Total Unidades]]</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="8" name="Horas semana" dataDxfId="9" dataCellStyle="Moneda"/>
-    <tableColumn id="12" name="Horas quincena" dataDxfId="8" dataCellStyle="Moneda"/>
-    <tableColumn id="13" name="Horas mes" dataDxfId="7" dataCellStyle="Moneda"/>
-    <tableColumn id="5" name="Total Horas" dataDxfId="6">
+    <tableColumn id="12" name="Horas quincena" dataDxfId="8" dataCellStyle="Moneda">
+      <calculatedColumnFormula>Tabla1[[#This Row],[Horas semana]]*2</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" name="Horas mes" dataDxfId="7" dataCellStyle="Moneda">
+      <calculatedColumnFormula>Tabla1[[#This Row],[Horas semana]]*4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" name="Total Horas" dataDxfId="13">
       <calculatedColumnFormula>Tabla1[Horas por Unidad]*Tabla1[Total Unidades]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Total Semanas" dataDxfId="5">
+    <tableColumn id="11" name="Total Semanas" dataDxfId="6">
       <calculatedColumnFormula>Tabla1[[#This Row],[Total Horas]]/Tabla1[[#This Row],[Horas semana]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Precio por hora" dataDxfId="4" dataCellStyle="Moneda"/>
-    <tableColumn id="6" name="Precio Total" dataDxfId="3" dataCellStyle="Moneda">
+    <tableColumn id="6" name="Precio Total" dataDxfId="5" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Total Horas]*Tabla1[Precio por hora]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Precio Semanal" dataDxfId="2" dataCellStyle="Moneda">
+    <tableColumn id="7" name="Precio Semanal" dataDxfId="12" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Mensual" dataDxfId="1" dataCellStyle="Moneda">
+    <tableColumn id="9" name="Mensual" dataDxfId="11" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Quincenal" dataDxfId="0" dataCellStyle="Moneda">
+    <tableColumn id="10" name="Quincenal" dataDxfId="10" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -874,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -885,17 +956,20 @@
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="4" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" customWidth="1"/>
-    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
-    <col min="11" max="11" width="14.77734375" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" customWidth="1"/>
+    <col min="13" max="13" width="10.109375" customWidth="1"/>
+    <col min="14" max="14" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -906,253 +980,274 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="2" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="18">
         <v>18</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="18">
         <v>8</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="1">
+        <f>Tabla1[[#This Row],[Total Semanas]]/Tabla1[[#This Row],[Total Unidades]]</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="16">
         <v>4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
+        <f>Tabla1[[#This Row],[Horas semana]]*2</f>
         <v>8</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
+        <f>Tabla1[[#This Row],[Horas semana]]*4</f>
         <v>16</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <f>Tabla1[Horas por Unidad]*Tabla1[Total Unidades]</f>
         <v>144</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <f>Tabla1[[#This Row],[Total Horas]]/Tabla1[[#This Row],[Horas semana]]</f>
         <v>36</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="17">
         <v>50</v>
       </c>
-      <c r="J2" s="4">
+      <c r="K2" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
         <v>7200</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
         <v>200</v>
       </c>
-      <c r="L2" s="4">
+      <c r="M2" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
         <v>800</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
         <v>400</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="18">
         <v>18</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="18">
         <v>8</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="1">
+        <f>Tabla1[[#This Row],[Total Semanas]]/Tabla1[[#This Row],[Total Unidades]]</f>
+        <v>2</v>
+      </c>
+      <c r="E3" s="16">
         <v>4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
+        <f>Tabla1[[#This Row],[Horas semana]]*2</f>
         <v>8</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
+        <f>Tabla1[[#This Row],[Horas semana]]*4</f>
         <v>16</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <f>Tabla1[Horas por Unidad]*Tabla1[Total Unidades]</f>
         <v>144</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <f>Tabla1[[#This Row],[Total Horas]]/Tabla1[[#This Row],[Horas semana]]</f>
         <v>36</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="17">
         <v>50</v>
       </c>
-      <c r="J3" s="4">
+      <c r="K3" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
         <v>7200</v>
       </c>
-      <c r="K3" s="4">
+      <c r="L3" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
         <v>200</v>
       </c>
-      <c r="L3" s="4">
+      <c r="M3" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
         <v>800</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
         <v>400</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="18">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="18">
         <v>8</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="1">
+        <f>Tabla1[[#This Row],[Total Semanas]]/Tabla1[[#This Row],[Total Unidades]]</f>
+        <v>2</v>
+      </c>
+      <c r="E4" s="16">
         <v>4</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
+        <f>Tabla1[[#This Row],[Horas semana]]*2</f>
         <v>8</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
+        <f>Tabla1[[#This Row],[Horas semana]]*4</f>
         <v>16</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f>Tabla1[Horas por Unidad]*Tabla1[Total Unidades]</f>
         <v>96</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <f>Tabla1[[#This Row],[Total Horas]]/Tabla1[[#This Row],[Horas semana]]</f>
         <v>24</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="17">
         <v>50</v>
       </c>
-      <c r="J4" s="4">
+      <c r="K4" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
         <v>4800</v>
       </c>
-      <c r="K4" s="4">
+      <c r="L4" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
         <v>200</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
         <v>800</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G8" s="7" t="s">
+    <row r="7" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="J8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="K8" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G9" s="10">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H9" s="10">
         <v>0.3</v>
       </c>
-      <c r="H9" s="6">
-        <f>J2-(L2*G9)</f>
+      <c r="I9" s="6">
+        <f>K2-(M2*H9)</f>
         <v>6960</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="11">
-        <f>J2-H9</f>
+      <c r="K9" s="11">
+        <f>K2-I9</f>
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G10" s="10">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H10" s="10">
         <v>0.2</v>
       </c>
-      <c r="H10" s="6">
-        <f>L2-(L3*G10)</f>
+      <c r="I10" s="6">
+        <f>M2-(M2*H10)</f>
         <v>640</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="11">
-        <f>L2-H10</f>
+      <c r="K10" s="11">
+        <f>M2-I10</f>
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="G11" s="10">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H11" s="10">
         <v>0.1</v>
       </c>
-      <c r="H11" s="6">
-        <f>M2-(M2*G11)</f>
+      <c r="I11" s="6">
+        <f>N2-(N2*H11)</f>
         <v>360</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="11">
-        <f>M2-H11</f>
+      <c r="K11" s="11">
+        <f>N2-I11</f>
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G12" s="12">
+    <row r="12" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="12">
         <v>0</v>
       </c>
-      <c r="H12" s="13">
-        <f>K2-(K2*G12)</f>
+      <c r="I12" s="13">
+        <f>L2-(L2*H12)</f>
         <v>200</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="J12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="15">
-        <f>K3-H12</f>
+      <c r="K12" s="15">
+        <f>L2-I12</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified courses price per hour. Payment logic code.
</commit_message>
<xml_diff>
--- a/admin/course_prices.xlsx
+++ b/admin/course_prices.xlsx
@@ -359,6 +359,62 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -383,6 +439,96 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Segoe UI"/>
+        <scheme val="none"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -418,19 +564,6 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -451,139 +584,6 @@
         <name val="Segoe UI"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Segoe UI"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -645,10 +645,10 @@
     <filterColumn colId="13" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="14">
-    <tableColumn id="1" name="Curso" dataDxfId="3"/>
-    <tableColumn id="2" name="Total Unidades" dataDxfId="2"/>
-    <tableColumn id="3" name="Horas por Unidad" dataDxfId="0"/>
-    <tableColumn id="14" name="Sem / unidad" dataDxfId="1">
+    <tableColumn id="1" name="Curso" dataDxfId="13"/>
+    <tableColumn id="2" name="Total Unidades" dataDxfId="12"/>
+    <tableColumn id="3" name="Horas por Unidad" dataDxfId="11"/>
+    <tableColumn id="14" name="Sem / unidad" dataDxfId="10">
       <calculatedColumnFormula>Tabla1[[#This Row],[Total Semanas]]/Tabla1[[#This Row],[Total Unidades]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="Horas semana" dataDxfId="9" dataCellStyle="Moneda"/>
@@ -658,23 +658,23 @@
     <tableColumn id="13" name="Horas mes" dataDxfId="7" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[[#This Row],[Horas semana]]*4</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Total Horas" dataDxfId="13">
+    <tableColumn id="5" name="Total Horas" dataDxfId="6">
       <calculatedColumnFormula>Tabla1[Horas por Unidad]*Tabla1[Total Unidades]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Total Semanas" dataDxfId="6">
+    <tableColumn id="11" name="Total Semanas" dataDxfId="5">
       <calculatedColumnFormula>Tabla1[[#This Row],[Total Horas]]/Tabla1[[#This Row],[Horas semana]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" name="Precio por hora" dataDxfId="4" dataCellStyle="Moneda"/>
-    <tableColumn id="6" name="Precio Total" dataDxfId="5" dataCellStyle="Moneda">
+    <tableColumn id="6" name="Precio Total" dataDxfId="3" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Total Horas]*Tabla1[Precio por hora]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Precio Semanal" dataDxfId="12" dataCellStyle="Moneda">
+    <tableColumn id="7" name="Precio Semanal" dataDxfId="2" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Mensual" dataDxfId="11" dataCellStyle="Moneda">
+    <tableColumn id="9" name="Mensual" dataDxfId="1" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Quincenal" dataDxfId="10" dataCellStyle="Moneda">
+    <tableColumn id="10" name="Quincenal" dataDxfId="0" dataCellStyle="Moneda">
       <calculatedColumnFormula>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -948,7 +948,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1047,23 +1047,23 @@
         <v>36</v>
       </c>
       <c r="J2" s="17">
-        <v>50</v>
+        <v>49.5</v>
       </c>
       <c r="K2" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
-        <v>7200</v>
+        <v>7128</v>
       </c>
       <c r="L2" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M2" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="N2" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -1100,23 +1100,23 @@
         <v>36</v>
       </c>
       <c r="J3" s="17">
-        <v>50</v>
+        <v>49.5</v>
       </c>
       <c r="K3" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
-        <v>7200</v>
+        <v>7128</v>
       </c>
       <c r="L3" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M3" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="N3" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -1153,23 +1153,23 @@
         <v>24</v>
       </c>
       <c r="J4" s="17">
-        <v>50</v>
+        <v>49.5</v>
       </c>
       <c r="K4" s="4">
         <f>Tabla1[Total Horas]*Tabla1[Precio por hora]</f>
-        <v>4800</v>
+        <v>4752</v>
       </c>
       <c r="L4" s="4">
         <f>Tabla1[[#This Row],[Precio por hora]]*Tabla1[[#This Row],[Horas semana]]</f>
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="M4" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas mes]]</f>
-        <v>800</v>
+        <v>792</v>
       </c>
       <c r="N4" s="4">
         <f>Tabla1[Precio por hora]*Tabla1[[#This Row],[Horas quincena]]</f>
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1193,14 +1193,14 @@
       </c>
       <c r="I9" s="6">
         <f>K2-(M2*H9)</f>
-        <v>6960</v>
+        <v>6890.4</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K9" s="11">
         <f>K2-I9</f>
-        <v>240</v>
+        <v>237.60000000000036</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
@@ -1209,14 +1209,14 @@
       </c>
       <c r="I10" s="6">
         <f>M2-(M2*H10)</f>
-        <v>640</v>
+        <v>633.6</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K10" s="11">
         <f>M2-I10</f>
-        <v>160</v>
+        <v>158.39999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
@@ -1225,14 +1225,14 @@
       </c>
       <c r="I11" s="6">
         <f>N2-(N2*H11)</f>
-        <v>360</v>
+        <v>356.4</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
       <c r="K11" s="11">
         <f>N2-I11</f>
-        <v>40</v>
+        <v>39.600000000000023</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="I12" s="13">
         <f>L2-(L2*H12)</f>
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J12" s="14" t="s">
         <v>10</v>

</xml_diff>